<commit_message>
Tested all of the cases
</commit_message>
<xml_diff>
--- a/12.17.20 - EG.xlsx
+++ b/12.17.20 - EG.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O2"/>
+  <dimension ref="A1:P2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -491,15 +491,20 @@
       </c>
       <c r="M1" s="1" t="inlineStr">
         <is>
+          <t>Gas Supplier</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
           <t>Gas Choice ID</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>Gas Rate Code</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>Gas Usage (therms)</t>
         </is>
@@ -566,15 +571,20 @@
       </c>
       <c r="M2" t="inlineStr">
         <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="N2" t="inlineStr">
+        <is>
           <t>5700075825</t>
         </is>
       </c>
-      <c r="N2" t="inlineStr">
+      <c r="O2" t="inlineStr">
         <is>
           <t>Schedule C</t>
         </is>
       </c>
-      <c r="O2" t="inlineStr">
+      <c r="P2" t="inlineStr">
         <is>
           <t>1612</t>
         </is>

</xml_diff>